<commit_message>
Fixed spaces in datafile
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -48,6 +48,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,9 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -398,20 +404,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G119" sqref="G119"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -425,7 +431,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>0.06</v>
       </c>
       <c r="B2" s="1">
@@ -439,7 +445,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>0.06</v>
       </c>
       <c r="B3" s="1">
@@ -453,7 +459,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>0.06</v>
       </c>
       <c r="B4" s="1">
@@ -467,7 +473,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>0.06</v>
       </c>
       <c r="B5" s="1">
@@ -481,7 +487,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>0.06</v>
       </c>
       <c r="B6" s="1">
@@ -495,7 +501,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>0.06</v>
       </c>
       <c r="B7" s="1">
@@ -509,7 +515,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>0.06</v>
       </c>
       <c r="B8" s="1">
@@ -523,7 +529,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>0.06</v>
       </c>
       <c r="B9" s="1">
@@ -537,7 +543,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>0.06</v>
       </c>
       <c r="B10" s="1">
@@ -551,7 +557,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>0.06</v>
       </c>
       <c r="B11" s="1">
@@ -565,7 +571,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>0.06</v>
       </c>
       <c r="B12" s="1">
@@ -579,7 +585,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>0.06</v>
       </c>
       <c r="B13" s="1">
@@ -593,7 +599,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>0.06</v>
       </c>
       <c r="B14" s="1">
@@ -607,7 +613,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>0.06</v>
       </c>
       <c r="B15" s="1">
@@ -621,7 +627,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>0.06</v>
       </c>
       <c r="B16" s="1">
@@ -635,7 +641,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>0.06</v>
       </c>
       <c r="B17" s="1">
@@ -649,7 +655,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>0.06</v>
       </c>
       <c r="B18" s="1">
@@ -663,7 +669,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>0.06</v>
       </c>
       <c r="B19" s="1">
@@ -677,7 +683,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>0.06</v>
       </c>
       <c r="B20" s="1">
@@ -691,7 +697,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>0.06</v>
       </c>
       <c r="B21" s="1">
@@ -705,7 +711,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>0.06</v>
       </c>
       <c r="B22" s="1">
@@ -719,7 +725,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>0.06</v>
       </c>
       <c r="B23" s="1">
@@ -733,7 +739,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>0.06</v>
       </c>
       <c r="B24" s="1">
@@ -747,7 +753,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>0.06</v>
       </c>
       <c r="B25" s="1">
@@ -761,7 +767,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>0.06</v>
       </c>
       <c r="B26" s="1">
@@ -775,7 +781,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>0.06</v>
       </c>
       <c r="B27" s="1">
@@ -789,7 +795,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>0.06</v>
       </c>
       <c r="B28" s="1">
@@ -803,7 +809,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>0.06</v>
       </c>
       <c r="B29" s="1">
@@ -817,7 +823,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>0.06</v>
       </c>
       <c r="B30" s="1">
@@ -831,7 +837,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>0.06</v>
       </c>
       <c r="B31" s="1">
@@ -845,7 +851,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>0.06</v>
       </c>
       <c r="B32" s="1">
@@ -859,7 +865,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>0.06</v>
       </c>
       <c r="B33" s="1">
@@ -873,7 +879,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>0.06</v>
       </c>
       <c r="B34" s="1">
@@ -887,7 +893,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>0.06</v>
       </c>
       <c r="B35" s="1">
@@ -901,7 +907,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>0.06</v>
       </c>
       <c r="B36" s="1">
@@ -915,7 +921,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>0.06</v>
       </c>
       <c r="B37" s="1">
@@ -929,7 +935,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>0.06</v>
       </c>
       <c r="B38" s="1">
@@ -943,7 +949,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>0.06</v>
       </c>
       <c r="B39" s="1">
@@ -957,7 +963,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>0.06</v>
       </c>
       <c r="B40" s="1">
@@ -971,7 +977,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>0.06</v>
       </c>
       <c r="B41" s="1">
@@ -985,7 +991,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B42" s="1">
@@ -999,7 +1005,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B43" s="1">
@@ -1013,7 +1019,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B44" s="1">
@@ -1027,7 +1033,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B45" s="1">
@@ -1041,7 +1047,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B46" s="1">
@@ -1055,7 +1061,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="A47" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B47" s="1">
@@ -1069,7 +1075,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B48" s="1">
@@ -1083,7 +1089,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B49" s="1">
@@ -1097,7 +1103,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B50" s="1">
@@ -1111,7 +1117,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B51" s="1">
@@ -1125,7 +1131,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B52" s="1">
@@ -1139,7 +1145,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B53" s="1">
@@ -1153,7 +1159,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B54" s="1">
@@ -1167,7 +1173,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B55" s="1">
@@ -1181,7 +1187,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B56" s="1">
@@ -1195,7 +1201,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B57" s="1">
@@ -1209,7 +1215,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B58" s="1">
@@ -1223,7 +1229,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B59" s="1">
@@ -1237,7 +1243,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B60" s="1">
@@ -1251,7 +1257,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B61" s="1">
@@ -1265,7 +1271,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="A62" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B62" s="1">
@@ -1279,7 +1285,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="A63" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B63" s="1">
@@ -1293,7 +1299,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="A64" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B64" s="1">
@@ -1307,7 +1313,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B65" s="1">
@@ -1321,7 +1327,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B66" s="1">
@@ -1335,7 +1341,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B67" s="1">
@@ -1349,7 +1355,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B68" s="1">
@@ -1363,7 +1369,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B69" s="1">
@@ -1377,7 +1383,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B70" s="1">
@@ -1391,7 +1397,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B71" s="1">
@@ -1405,7 +1411,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+      <c r="A72" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B72" s="1">
@@ -1419,7 +1425,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="A73" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B73" s="1">
@@ -1433,7 +1439,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+      <c r="A74" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B74" s="1">
@@ -1447,7 +1453,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B75" s="1">
@@ -1461,7 +1467,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="A76" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B76" s="1">
@@ -1475,7 +1481,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="A77" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B77" s="1">
@@ -1489,7 +1495,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+      <c r="A78" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B78" s="1">
@@ -1503,7 +1509,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="A79" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B79" s="1">
@@ -1517,7 +1523,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="A80" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B80" s="1">
@@ -1531,7 +1537,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+      <c r="A81" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B81" s="1">
@@ -1545,7 +1551,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="A82" s="2">
         <v>0.08</v>
       </c>
       <c r="B82" s="1">
@@ -1559,7 +1565,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83" s="2">
         <v>0.08</v>
       </c>
       <c r="B83" s="1">
@@ -1573,7 +1579,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+      <c r="A84" s="2">
         <v>0.08</v>
       </c>
       <c r="B84" s="1">
@@ -1587,7 +1593,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="A85" s="2">
         <v>0.08</v>
       </c>
       <c r="B85" s="1">
@@ -1601,7 +1607,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+      <c r="A86" s="2">
         <v>0.08</v>
       </c>
       <c r="B86" s="1">
@@ -1615,7 +1621,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="A87" s="2">
         <v>0.08</v>
       </c>
       <c r="B87" s="1">
@@ -1629,7 +1635,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+      <c r="A88" s="2">
         <v>0.08</v>
       </c>
       <c r="B88" s="1">
@@ -1643,7 +1649,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+      <c r="A89" s="2">
         <v>0.08</v>
       </c>
       <c r="B89" s="1">
@@ -1657,7 +1663,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+      <c r="A90" s="2">
         <v>0.08</v>
       </c>
       <c r="B90" s="1">
@@ -1671,7 +1677,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="A91" s="2">
         <v>0.08</v>
       </c>
       <c r="B91" s="1">
@@ -1685,7 +1691,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="A92" s="2">
         <v>0.08</v>
       </c>
       <c r="B92" s="1">
@@ -1699,7 +1705,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+      <c r="A93" s="2">
         <v>0.08</v>
       </c>
       <c r="B93" s="1">
@@ -1713,7 +1719,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+      <c r="A94" s="2">
         <v>0.08</v>
       </c>
       <c r="B94" s="1">
@@ -1727,7 +1733,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="A95" s="2">
         <v>0.08</v>
       </c>
       <c r="B95" s="1">
@@ -1741,7 +1747,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="A96" s="2">
         <v>0.08</v>
       </c>
       <c r="B96" s="1">
@@ -1755,7 +1761,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="A97" s="2">
         <v>0.08</v>
       </c>
       <c r="B97" s="1">
@@ -1769,7 +1775,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+      <c r="A98" s="2">
         <v>0.08</v>
       </c>
       <c r="B98" s="1">
@@ -1783,7 +1789,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+      <c r="A99" s="2">
         <v>0.08</v>
       </c>
       <c r="B99" s="1">
@@ -1797,7 +1803,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+      <c r="A100" s="2">
         <v>0.08</v>
       </c>
       <c r="B100" s="1">
@@ -1811,7 +1817,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+      <c r="A101" s="2">
         <v>0.08</v>
       </c>
       <c r="B101" s="1">
@@ -1825,7 +1831,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+      <c r="A102" s="2">
         <v>0.08</v>
       </c>
       <c r="B102" s="1">
@@ -1839,7 +1845,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+      <c r="A103" s="2">
         <v>0.08</v>
       </c>
       <c r="B103" s="1">
@@ -1853,7 +1859,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+      <c r="A104" s="2">
         <v>0.08</v>
       </c>
       <c r="B104" s="1">
@@ -1867,7 +1873,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+      <c r="A105" s="2">
         <v>0.08</v>
       </c>
       <c r="B105" s="1">
@@ -1881,7 +1887,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+      <c r="A106" s="2">
         <v>0.08</v>
       </c>
       <c r="B106" s="1">
@@ -1895,7 +1901,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+      <c r="A107" s="2">
         <v>0.08</v>
       </c>
       <c r="B107" s="1">
@@ -1909,7 +1915,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+      <c r="A108" s="2">
         <v>0.08</v>
       </c>
       <c r="B108" s="1">
@@ -1923,7 +1929,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+      <c r="A109" s="2">
         <v>0.08</v>
       </c>
       <c r="B109" s="1">
@@ -1937,7 +1943,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+      <c r="A110" s="2">
         <v>0.08</v>
       </c>
       <c r="B110" s="1">
@@ -1951,7 +1957,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+      <c r="A111" s="2">
         <v>0.08</v>
       </c>
       <c r="B111" s="1">
@@ -1965,7 +1971,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+      <c r="A112" s="2">
         <v>0.08</v>
       </c>
       <c r="B112" s="1">
@@ -1979,7 +1985,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+      <c r="A113" s="2">
         <v>0.08</v>
       </c>
       <c r="B113" s="1">
@@ -1993,7 +1999,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+      <c r="A114" s="2">
         <v>0.08</v>
       </c>
       <c r="B114" s="1">
@@ -2007,7 +2013,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+      <c r="A115" s="2">
         <v>0.08</v>
       </c>
       <c r="B115" s="1">
@@ -2021,7 +2027,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+      <c r="A116" s="2">
         <v>0.08</v>
       </c>
       <c r="B116" s="1">
@@ -2035,7 +2041,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+      <c r="A117" s="2">
         <v>0.08</v>
       </c>
       <c r="B117" s="1">
@@ -2049,7 +2055,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+      <c r="A118" s="2">
         <v>0.08</v>
       </c>
       <c r="B118" s="1">
@@ -2063,7 +2069,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+      <c r="A119" s="2">
         <v>0.08</v>
       </c>
       <c r="B119" s="1">
@@ -2077,7 +2083,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
+      <c r="A120" s="2">
         <v>0.08</v>
       </c>
       <c r="B120" s="1">
@@ -2091,7 +2097,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+      <c r="A121" s="2">
         <v>0.08</v>
       </c>
       <c r="B121" s="1">
@@ -2105,7 +2111,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
+      <c r="A122" s="2">
         <v>0.09</v>
       </c>
       <c r="B122" s="1">
@@ -2119,7 +2125,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+      <c r="A123" s="2">
         <v>0.09</v>
       </c>
       <c r="B123" s="1">
@@ -2133,7 +2139,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
+      <c r="A124" s="2">
         <v>0.09</v>
       </c>
       <c r="B124" s="1">
@@ -2147,7 +2153,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
+      <c r="A125" s="2">
         <v>0.09</v>
       </c>
       <c r="B125" s="1">
@@ -2161,7 +2167,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+      <c r="A126" s="2">
         <v>0.09</v>
       </c>
       <c r="B126" s="1">
@@ -2175,7 +2181,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+      <c r="A127" s="2">
         <v>0.09</v>
       </c>
       <c r="B127" s="1">
@@ -2189,7 +2195,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
+      <c r="A128" s="2">
         <v>0.09</v>
       </c>
       <c r="B128" s="1">
@@ -2203,7 +2209,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
+      <c r="A129" s="2">
         <v>0.09</v>
       </c>
       <c r="B129" s="1">
@@ -2217,7 +2223,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
+      <c r="A130" s="2">
         <v>0.09</v>
       </c>
       <c r="B130" s="1">
@@ -2231,7 +2237,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
+      <c r="A131" s="2">
         <v>0.09</v>
       </c>
       <c r="B131" s="1">
@@ -2245,7 +2251,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
+      <c r="A132" s="2">
         <v>0.09</v>
       </c>
       <c r="B132" s="1">
@@ -2259,7 +2265,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
+      <c r="A133" s="2">
         <v>0.09</v>
       </c>
       <c r="B133" s="1">
@@ -2273,7 +2279,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
+      <c r="A134" s="2">
         <v>0.09</v>
       </c>
       <c r="B134" s="1">
@@ -2287,7 +2293,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
+      <c r="A135" s="2">
         <v>0.09</v>
       </c>
       <c r="B135" s="1">
@@ -2301,7 +2307,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
+      <c r="A136" s="2">
         <v>0.09</v>
       </c>
       <c r="B136" s="1">
@@ -2315,7 +2321,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
+      <c r="A137" s="2">
         <v>0.09</v>
       </c>
       <c r="B137" s="1">
@@ -2329,7 +2335,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
+      <c r="A138" s="2">
         <v>0.09</v>
       </c>
       <c r="B138" s="1">
@@ -2343,7 +2349,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
+      <c r="A139" s="2">
         <v>0.09</v>
       </c>
       <c r="B139" s="1">
@@ -2357,7 +2363,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
+      <c r="A140" s="2">
         <v>0.09</v>
       </c>
       <c r="B140" s="1">
@@ -2371,7 +2377,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
+      <c r="A141" s="2">
         <v>0.09</v>
       </c>
       <c r="B141" s="1">
@@ -2385,7 +2391,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
+      <c r="A142" s="2">
         <v>0.09</v>
       </c>
       <c r="B142" s="1">
@@ -2399,7 +2405,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+      <c r="A143" s="2">
         <v>0.09</v>
       </c>
       <c r="B143" s="1">
@@ -2413,7 +2419,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
+      <c r="A144" s="2">
         <v>0.09</v>
       </c>
       <c r="B144" s="1">
@@ -2427,7 +2433,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
+      <c r="A145" s="2">
         <v>0.09</v>
       </c>
       <c r="B145" s="1">
@@ -2441,7 +2447,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
+      <c r="A146" s="2">
         <v>0.09</v>
       </c>
       <c r="B146" s="1">
@@ -2455,7 +2461,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
+      <c r="A147" s="2">
         <v>0.09</v>
       </c>
       <c r="B147" s="1">
@@ -2469,7 +2475,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
+      <c r="A148" s="2">
         <v>0.09</v>
       </c>
       <c r="B148" s="1">
@@ -2483,7 +2489,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
+      <c r="A149" s="2">
         <v>0.09</v>
       </c>
       <c r="B149" s="1">
@@ -2497,7 +2503,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
+      <c r="A150" s="2">
         <v>0.09</v>
       </c>
       <c r="B150" s="1">
@@ -2511,7 +2517,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
+      <c r="A151" s="2">
         <v>0.09</v>
       </c>
       <c r="B151" s="1">
@@ -2525,7 +2531,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
+      <c r="A152" s="2">
         <v>0.09</v>
       </c>
       <c r="B152" s="1">
@@ -2539,7 +2545,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
+      <c r="A153" s="2">
         <v>0.09</v>
       </c>
       <c r="B153" s="1">
@@ -2553,7 +2559,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
+      <c r="A154" s="2">
         <v>0.09</v>
       </c>
       <c r="B154" s="1">
@@ -2567,7 +2573,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
+      <c r="A155" s="2">
         <v>0.09</v>
       </c>
       <c r="B155" s="1">
@@ -2581,7 +2587,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
+      <c r="A156" s="2">
         <v>0.09</v>
       </c>
       <c r="B156" s="1">
@@ -2595,7 +2601,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
+      <c r="A157" s="2">
         <v>0.09</v>
       </c>
       <c r="B157" s="1">
@@ -2609,7 +2615,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
+      <c r="A158" s="2">
         <v>0.09</v>
       </c>
       <c r="B158" s="1">
@@ -2623,7 +2629,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
+      <c r="A159" s="2">
         <v>0.09</v>
       </c>
       <c r="B159" s="1">
@@ -2637,7 +2643,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
+      <c r="A160" s="2">
         <v>0.09</v>
       </c>
       <c r="B160" s="1">
@@ -2651,7 +2657,7 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
+      <c r="A161" s="2">
         <v>0.09</v>
       </c>
       <c r="B161" s="1">
@@ -2665,7 +2671,7 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
+      <c r="A162" s="2">
         <v>0.1</v>
       </c>
       <c r="B162" s="1">
@@ -2679,7 +2685,7 @@
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
+      <c r="A163" s="2">
         <v>0.1</v>
       </c>
       <c r="B163" s="1">
@@ -2693,7 +2699,7 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
+      <c r="A164" s="2">
         <v>0.1</v>
       </c>
       <c r="B164" s="1">
@@ -2707,7 +2713,7 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
+      <c r="A165" s="2">
         <v>0.1</v>
       </c>
       <c r="B165" s="1">
@@ -2721,7 +2727,7 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
+      <c r="A166" s="2">
         <v>0.1</v>
       </c>
       <c r="B166" s="1">
@@ -2735,7 +2741,7 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
+      <c r="A167" s="2">
         <v>0.1</v>
       </c>
       <c r="B167" s="1">
@@ -2749,7 +2755,7 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
+      <c r="A168" s="2">
         <v>0.1</v>
       </c>
       <c r="B168" s="1">
@@ -2763,7 +2769,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
+      <c r="A169" s="2">
         <v>0.1</v>
       </c>
       <c r="B169" s="1">
@@ -2777,7 +2783,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
+      <c r="A170" s="2">
         <v>0.1</v>
       </c>
       <c r="B170" s="1">
@@ -2791,7 +2797,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
+      <c r="A171" s="2">
         <v>0.1</v>
       </c>
       <c r="B171" s="1">
@@ -2805,7 +2811,7 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
+      <c r="A172" s="2">
         <v>0.1</v>
       </c>
       <c r="B172" s="1">
@@ -2819,7 +2825,7 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
+      <c r="A173" s="2">
         <v>0.1</v>
       </c>
       <c r="B173" s="1">
@@ -2833,7 +2839,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
+      <c r="A174" s="2">
         <v>0.1</v>
       </c>
       <c r="B174" s="1">
@@ -2847,7 +2853,7 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
+      <c r="A175" s="2">
         <v>0.1</v>
       </c>
       <c r="B175" s="1">
@@ -2861,7 +2867,7 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
+      <c r="A176" s="2">
         <v>0.1</v>
       </c>
       <c r="B176" s="1">
@@ -2875,7 +2881,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
+      <c r="A177" s="2">
         <v>0.1</v>
       </c>
       <c r="B177" s="1">
@@ -2889,7 +2895,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
+      <c r="A178" s="2">
         <v>0.1</v>
       </c>
       <c r="B178" s="1">
@@ -2903,7 +2909,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
+      <c r="A179" s="2">
         <v>0.1</v>
       </c>
       <c r="B179" s="1">
@@ -2917,7 +2923,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
+      <c r="A180" s="2">
         <v>0.1</v>
       </c>
       <c r="B180" s="1">
@@ -2931,7 +2937,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
+      <c r="A181" s="2">
         <v>0.1</v>
       </c>
       <c r="B181" s="1">
@@ -2945,7 +2951,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
+      <c r="A182" s="2">
         <v>0.1</v>
       </c>
       <c r="B182" s="1">
@@ -2959,7 +2965,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
+      <c r="A183" s="2">
         <v>0.1</v>
       </c>
       <c r="B183" s="1">
@@ -2973,7 +2979,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
+      <c r="A184" s="2">
         <v>0.1</v>
       </c>
       <c r="B184" s="1">
@@ -2987,7 +2993,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
+      <c r="A185" s="2">
         <v>0.1</v>
       </c>
       <c r="B185" s="1">
@@ -3001,7 +3007,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
+      <c r="A186" s="2">
         <v>0.1</v>
       </c>
       <c r="B186" s="1">
@@ -3015,7 +3021,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
+      <c r="A187" s="2">
         <v>0.1</v>
       </c>
       <c r="B187" s="1">
@@ -3029,7 +3035,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
+      <c r="A188" s="2">
         <v>0.1</v>
       </c>
       <c r="B188" s="1">
@@ -3043,7 +3049,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
+      <c r="A189" s="2">
         <v>0.1</v>
       </c>
       <c r="B189" s="1">
@@ -3057,7 +3063,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
+      <c r="A190" s="2">
         <v>0.1</v>
       </c>
       <c r="B190" s="1">
@@ -3071,7 +3077,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
+      <c r="A191" s="2">
         <v>0.1</v>
       </c>
       <c r="B191" s="1">
@@ -3085,7 +3091,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
+      <c r="A192" s="2">
         <v>0.1</v>
       </c>
       <c r="B192" s="1">
@@ -3099,7 +3105,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
+      <c r="A193" s="2">
         <v>0.1</v>
       </c>
       <c r="B193" s="1">
@@ -3113,7 +3119,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
+      <c r="A194" s="2">
         <v>0.1</v>
       </c>
       <c r="B194" s="1">
@@ -3127,7 +3133,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
+      <c r="A195" s="2">
         <v>0.1</v>
       </c>
       <c r="B195" s="1">
@@ -3141,7 +3147,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
+      <c r="A196" s="2">
         <v>0.1</v>
       </c>
       <c r="B196" s="1">
@@ -3155,7 +3161,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
+      <c r="A197" s="2">
         <v>0.1</v>
       </c>
       <c r="B197" s="1">
@@ -3169,7 +3175,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
+      <c r="A198" s="2">
         <v>0.1</v>
       </c>
       <c r="B198" s="1">
@@ -3183,7 +3189,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
+      <c r="A199" s="2">
         <v>0.1</v>
       </c>
       <c r="B199" s="1">
@@ -3197,7 +3203,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
+      <c r="A200" s="2">
         <v>0.1</v>
       </c>
       <c r="B200" s="1">
@@ -3211,7 +3217,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
+      <c r="A201" s="2">
         <v>0.1</v>
       </c>
       <c r="B201" s="1">
@@ -3225,7 +3231,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
+      <c r="A202" s="2">
         <v>0.11</v>
       </c>
       <c r="B202" s="1">
@@ -3239,7 +3245,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
+      <c r="A203" s="2">
         <v>0.11</v>
       </c>
       <c r="B203" s="1">
@@ -3253,7 +3259,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
+      <c r="A204" s="2">
         <v>0.11</v>
       </c>
       <c r="B204" s="1">
@@ -3267,7 +3273,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="1">
+      <c r="A205" s="2">
         <v>0.11</v>
       </c>
       <c r="B205" s="1">
@@ -3281,7 +3287,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="1">
+      <c r="A206" s="2">
         <v>0.11</v>
       </c>
       <c r="B206" s="1">
@@ -3295,7 +3301,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="1">
+      <c r="A207" s="2">
         <v>0.11</v>
       </c>
       <c r="B207" s="1">
@@ -3309,7 +3315,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
+      <c r="A208" s="2">
         <v>0.11</v>
       </c>
       <c r="B208" s="1">
@@ -3323,7 +3329,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
+      <c r="A209" s="2">
         <v>0.11</v>
       </c>
       <c r="B209" s="1">
@@ -3337,7 +3343,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="1">
+      <c r="A210" s="2">
         <v>0.11</v>
       </c>
       <c r="B210" s="1">
@@ -3351,7 +3357,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
+      <c r="A211" s="2">
         <v>0.11</v>
       </c>
       <c r="B211" s="1">
@@ -3365,7 +3371,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
+      <c r="A212" s="2">
         <v>0.11</v>
       </c>
       <c r="B212" s="1">
@@ -3379,7 +3385,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="1">
+      <c r="A213" s="2">
         <v>0.11</v>
       </c>
       <c r="B213" s="1">
@@ -3393,7 +3399,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="1">
+      <c r="A214" s="2">
         <v>0.11</v>
       </c>
       <c r="B214" s="1">
@@ -3407,7 +3413,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="1">
+      <c r="A215" s="2">
         <v>0.11</v>
       </c>
       <c r="B215" s="1">
@@ -3421,7 +3427,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
+      <c r="A216" s="2">
         <v>0.11</v>
       </c>
       <c r="B216" s="1">
@@ -3435,7 +3441,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="1">
+      <c r="A217" s="2">
         <v>0.11</v>
       </c>
       <c r="B217" s="1">
@@ -3449,7 +3455,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="1">
+      <c r="A218" s="2">
         <v>0.11</v>
       </c>
       <c r="B218" s="1">
@@ -3463,7 +3469,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
+      <c r="A219" s="2">
         <v>0.11</v>
       </c>
       <c r="B219" s="1">
@@ -3477,7 +3483,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="1">
+      <c r="A220" s="2">
         <v>0.11</v>
       </c>
       <c r="B220" s="1">
@@ -3491,7 +3497,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="1">
+      <c r="A221" s="2">
         <v>0.11</v>
       </c>
       <c r="B221" s="1">
@@ -3505,7 +3511,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="1">
+      <c r="A222" s="2">
         <v>0.11</v>
       </c>
       <c r="B222" s="1">
@@ -3519,7 +3525,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="1">
+      <c r="A223" s="2">
         <v>0.11</v>
       </c>
       <c r="B223" s="1">
@@ -3533,7 +3539,7 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="1">
+      <c r="A224" s="2">
         <v>0.11</v>
       </c>
       <c r="B224" s="1">
@@ -3547,7 +3553,7 @@
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="1">
+      <c r="A225" s="2">
         <v>0.11</v>
       </c>
       <c r="B225" s="1">
@@ -3561,7 +3567,7 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="1">
+      <c r="A226" s="2">
         <v>0.11</v>
       </c>
       <c r="B226" s="1">
@@ -3575,7 +3581,7 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="1">
+      <c r="A227" s="2">
         <v>0.11</v>
       </c>
       <c r="B227" s="1">
@@ -3589,7 +3595,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="1">
+      <c r="A228" s="2">
         <v>0.11</v>
       </c>
       <c r="B228" s="1">
@@ -3603,7 +3609,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
+      <c r="A229" s="2">
         <v>0.11</v>
       </c>
       <c r="B229" s="1">
@@ -3617,7 +3623,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="1">
+      <c r="A230" s="2">
         <v>0.11</v>
       </c>
       <c r="B230" s="1">
@@ -3631,7 +3637,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="1">
+      <c r="A231" s="2">
         <v>0.11</v>
       </c>
       <c r="B231" s="1">
@@ -3645,7 +3651,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="1">
+      <c r="A232" s="2">
         <v>0.11</v>
       </c>
       <c r="B232" s="1">
@@ -3659,7 +3665,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
+      <c r="A233" s="2">
         <v>0.11</v>
       </c>
       <c r="B233" s="1">
@@ -3673,7 +3679,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="1">
+      <c r="A234" s="2">
         <v>0.11</v>
       </c>
       <c r="B234" s="1">
@@ -3687,7 +3693,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="1">
+      <c r="A235" s="2">
         <v>0.11</v>
       </c>
       <c r="B235" s="1">
@@ -3701,7 +3707,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="1">
+      <c r="A236" s="2">
         <v>0.11</v>
       </c>
       <c r="B236" s="1">
@@ -3715,7 +3721,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="1">
+      <c r="A237" s="2">
         <v>0.11</v>
       </c>
       <c r="B237" s="1">
@@ -3729,7 +3735,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="1">
+      <c r="A238" s="2">
         <v>0.11</v>
       </c>
       <c r="B238" s="1">
@@ -3743,7 +3749,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="1">
+      <c r="A239" s="2">
         <v>0.11</v>
       </c>
       <c r="B239" s="1">
@@ -3757,7 +3763,7 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="1">
+      <c r="A240" s="2">
         <v>0.11</v>
       </c>
       <c r="B240" s="1">
@@ -3771,7 +3777,7 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="1">
+      <c r="A241" s="2">
         <v>0.11</v>
       </c>
       <c r="B241" s="1">
@@ -3786,5 +3792,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>